<commit_message>
chl comparisions and senescence recording updated
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025-231_Senescence.xlsx
+++ b/data/monitoringPhenology/2025-231_Senescence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D756FD79-0FB5-6A43-80FC-A4D235175E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE8F850-80D2-604B-9E6C-039FE5EB57DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="468">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1440,6 +1440,9 @@
   </si>
   <si>
     <t>only 4 leaves, very small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2182,7 +2185,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2297,14 +2300,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}" name="Table1" displayName="Table1" ref="A1:M437" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="A1:M437" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="3"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="betula"/>
+        <filter val="acer"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2649,7 +2647,7 @@
     <sheetView tabSelected="1" zoomScale="207" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A493" sqref="A493"/>
-      <selection pane="topRight" activeCell="K166" sqref="K166"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2702,107 +2700,167 @@
         <v>464</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G2" s="1">
+        <v>231</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30.2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>25.2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G3" s="1">
+        <v>231</v>
+      </c>
+      <c r="H3" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="I3" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>29.5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G4" s="1">
+        <v>231</v>
+      </c>
+      <c r="H4" s="1">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1">
+        <v>29</v>
+      </c>
+      <c r="K4" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G5" s="1">
+        <v>231</v>
+      </c>
+      <c r="H5" s="1">
+        <v>31.7</v>
+      </c>
+      <c r="I5" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="1">
+        <v>231</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2821,8 +2879,20 @@
       <c r="G7">
         <v>231</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>23.8</v>
+      </c>
+      <c r="J7">
+        <v>29.1</v>
+      </c>
+      <c r="K7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2841,8 +2911,20 @@
       <c r="G8">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>26.7</v>
+      </c>
+      <c r="I8">
+        <v>23.9</v>
+      </c>
+      <c r="J8">
+        <v>26.6</v>
+      </c>
+      <c r="K8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2861,8 +2943,20 @@
       <c r="G9">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>15.8</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>24.1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2881,8 +2975,20 @@
       <c r="G10">
         <v>231</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>20.9</v>
+      </c>
+      <c r="I10">
+        <v>21.8</v>
+      </c>
+      <c r="J10">
+        <v>15.9</v>
+      </c>
+      <c r="K10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2901,8 +3007,20 @@
       <c r="G11">
         <v>231</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>17.3</v>
+      </c>
+      <c r="I11">
+        <v>26.3</v>
+      </c>
+      <c r="J11">
+        <v>16.3</v>
+      </c>
+      <c r="K11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2921,8 +3039,20 @@
       <c r="G12">
         <v>231</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>27.8</v>
+      </c>
+      <c r="I12">
+        <v>25.4</v>
+      </c>
+      <c r="J12">
+        <v>29.7</v>
+      </c>
+      <c r="K12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2941,8 +3071,20 @@
       <c r="G13">
         <v>231</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>28.3</v>
+      </c>
+      <c r="I13">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="J13">
+        <v>24.7</v>
+      </c>
+      <c r="K13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2961,8 +3103,20 @@
       <c r="G14">
         <v>231</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>25.1</v>
+      </c>
+      <c r="I14">
+        <v>23.8</v>
+      </c>
+      <c r="J14">
+        <v>20.3</v>
+      </c>
+      <c r="K14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2981,8 +3135,20 @@
       <c r="G15">
         <v>231</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>28.5</v>
+      </c>
+      <c r="I15">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="J15">
+        <v>25.6</v>
+      </c>
+      <c r="K15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3001,8 +3167,20 @@
       <c r="G16">
         <v>231</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I16">
+        <v>24.2</v>
+      </c>
+      <c r="J16">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="K16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3021,8 +3199,20 @@
       <c r="G17">
         <v>231</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>18.7</v>
+      </c>
+      <c r="I17">
+        <v>26.6</v>
+      </c>
+      <c r="J17">
+        <v>22.1</v>
+      </c>
+      <c r="K17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3041,8 +3231,20 @@
       <c r="G18">
         <v>231</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="I18" s="1">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3061,8 +3263,20 @@
       <c r="G19">
         <v>231</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <v>28.5</v>
+      </c>
+      <c r="I19" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="K19" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3081,8 +3295,20 @@
       <c r="G20">
         <v>231</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <v>15.9</v>
+      </c>
+      <c r="I20" s="1">
+        <v>31</v>
+      </c>
+      <c r="J20" s="1">
+        <v>24</v>
+      </c>
+      <c r="K20" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3101,8 +3327,20 @@
       <c r="G21">
         <v>231</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="I21">
+        <v>23.1</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3121,8 +3359,20 @@
       <c r="G22">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I22">
+        <v>10.7</v>
+      </c>
+      <c r="J22">
+        <v>21.4</v>
+      </c>
+      <c r="K22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3141,8 +3391,20 @@
       <c r="G23">
         <v>231</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>17</v>
+      </c>
+      <c r="I23">
+        <v>20.2</v>
+      </c>
+      <c r="J23">
+        <v>27</v>
+      </c>
+      <c r="K23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3161,8 +3423,20 @@
       <c r="G24">
         <v>231</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>18.3</v>
+      </c>
+      <c r="I24">
+        <v>22.2</v>
+      </c>
+      <c r="J24">
+        <v>23</v>
+      </c>
+      <c r="K24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3181,8 +3455,20 @@
       <c r="G25">
         <v>231</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>13.6</v>
+      </c>
+      <c r="I25">
+        <v>21.4</v>
+      </c>
+      <c r="J25">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3201,8 +3487,20 @@
       <c r="G26">
         <v>231</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>20.3</v>
+      </c>
+      <c r="I26">
+        <v>15.8</v>
+      </c>
+      <c r="J26">
+        <v>24.7</v>
+      </c>
+      <c r="K26">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3221,8 +3519,20 @@
       <c r="G27">
         <v>231</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>27.3</v>
+      </c>
+      <c r="I27">
+        <v>20.2</v>
+      </c>
+      <c r="J27">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3241,8 +3551,20 @@
       <c r="G28">
         <v>231</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>30.5</v>
+      </c>
+      <c r="I28">
+        <v>29.3</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
+      <c r="K28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3261,8 +3583,20 @@
       <c r="G29">
         <v>231</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>27.9</v>
+      </c>
+      <c r="I29">
+        <v>33.4</v>
+      </c>
+      <c r="J29">
+        <v>33.9</v>
+      </c>
+      <c r="K29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -3281,8 +3615,20 @@
       <c r="G30">
         <v>231</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I30">
+        <v>28.6</v>
+      </c>
+      <c r="J30">
+        <v>24.5</v>
+      </c>
+      <c r="K30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3301,8 +3647,20 @@
       <c r="G31">
         <v>231</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>12.2</v>
+      </c>
+      <c r="I31">
+        <v>29.7</v>
+      </c>
+      <c r="J31">
+        <v>26.7</v>
+      </c>
+      <c r="K31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -3321,8 +3679,20 @@
       <c r="G32">
         <v>231</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>25.2</v>
+      </c>
+      <c r="I32">
+        <v>27.5</v>
+      </c>
+      <c r="J32">
+        <v>20</v>
+      </c>
+      <c r="K32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -3341,8 +3711,20 @@
       <c r="G33">
         <v>231</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>25.5</v>
+      </c>
+      <c r="I33">
+        <v>28.1</v>
+      </c>
+      <c r="J33">
+        <v>31.8</v>
+      </c>
+      <c r="K33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3361,8 +3743,20 @@
       <c r="G34">
         <v>231</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>31.5</v>
+      </c>
+      <c r="I34">
+        <v>26.6</v>
+      </c>
+      <c r="J34">
+        <v>25.4</v>
+      </c>
+      <c r="K34">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -3381,8 +3775,20 @@
       <c r="G35">
         <v>231</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>21.5</v>
+      </c>
+      <c r="I35">
+        <v>28.4</v>
+      </c>
+      <c r="J35">
+        <v>23.5</v>
+      </c>
+      <c r="K35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3401,8 +3807,20 @@
       <c r="G36">
         <v>231</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>31.3</v>
+      </c>
+      <c r="I36">
+        <v>37.4</v>
+      </c>
+      <c r="J36">
+        <v>30.8</v>
+      </c>
+      <c r="K36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3421,8 +3839,20 @@
       <c r="G37">
         <v>231</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>19.2</v>
+      </c>
+      <c r="I37">
+        <v>22.6</v>
+      </c>
+      <c r="J37">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="K37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3441,8 +3871,20 @@
       <c r="G38">
         <v>231</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>22</v>
+      </c>
+      <c r="I38">
+        <v>27.8</v>
+      </c>
+      <c r="J38">
+        <v>22.5</v>
+      </c>
+      <c r="K38">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3461,8 +3903,20 @@
       <c r="G39">
         <v>231</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I39">
+        <v>22.2</v>
+      </c>
+      <c r="J39">
+        <v>21.5</v>
+      </c>
+      <c r="K39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3481,8 +3935,20 @@
       <c r="G40">
         <v>231</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I40">
+        <v>26.8</v>
+      </c>
+      <c r="J40">
+        <v>23.3</v>
+      </c>
+      <c r="K40">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3501,8 +3967,20 @@
       <c r="G41">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>13.8</v>
+      </c>
+      <c r="I41">
+        <v>13.6</v>
+      </c>
+      <c r="J41">
+        <v>15.3</v>
+      </c>
+      <c r="K41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3521,8 +3999,20 @@
       <c r="G42">
         <v>231</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="I42">
+        <v>26.4</v>
+      </c>
+      <c r="J42">
+        <v>27.7</v>
+      </c>
+      <c r="K42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3541,8 +4031,20 @@
       <c r="G43">
         <v>231</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>27.2</v>
+      </c>
+      <c r="I43">
+        <v>24.6</v>
+      </c>
+      <c r="J43">
+        <v>25.5</v>
+      </c>
+      <c r="K43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3561,8 +4063,20 @@
       <c r="G44">
         <v>231</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>26.4</v>
+      </c>
+      <c r="I44">
+        <v>15.5</v>
+      </c>
+      <c r="J44">
+        <v>28.3</v>
+      </c>
+      <c r="K44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3581,8 +4095,20 @@
       <c r="G45">
         <v>231</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>21.5</v>
+      </c>
+      <c r="I45">
+        <v>27.3</v>
+      </c>
+      <c r="J45">
+        <v>29.2</v>
+      </c>
+      <c r="K45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3601,8 +4127,20 @@
       <c r="G46">
         <v>231</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>34.4</v>
+      </c>
+      <c r="I46">
+        <v>33.5</v>
+      </c>
+      <c r="J46">
+        <v>38.6</v>
+      </c>
+      <c r="K46">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3621,8 +4159,20 @@
       <c r="G47">
         <v>231</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I47">
+        <v>24.6</v>
+      </c>
+      <c r="J47">
+        <v>34</v>
+      </c>
+      <c r="K47">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -3641,8 +4191,20 @@
       <c r="G48">
         <v>231</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>22.6</v>
+      </c>
+      <c r="I48">
+        <v>25.2</v>
+      </c>
+      <c r="J48">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="K48">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -3661,8 +4223,20 @@
       <c r="G49">
         <v>231</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>19.5</v>
+      </c>
+      <c r="I49">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J49">
+        <v>25.1</v>
+      </c>
+      <c r="K49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -3681,8 +4255,20 @@
       <c r="G50">
         <v>231</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>22.8</v>
+      </c>
+      <c r="I50">
+        <v>20.9</v>
+      </c>
+      <c r="J50">
+        <v>27.2</v>
+      </c>
+      <c r="K50">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -3701,8 +4287,20 @@
       <c r="G51">
         <v>231</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>25.8</v>
+      </c>
+      <c r="I51">
+        <v>25.1</v>
+      </c>
+      <c r="J51">
+        <v>17.8</v>
+      </c>
+      <c r="K51">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -3721,8 +4319,20 @@
       <c r="G52">
         <v>231</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>22.1</v>
+      </c>
+      <c r="I52">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J52">
+        <v>29.4</v>
+      </c>
+      <c r="K52">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -3741,8 +4351,20 @@
       <c r="G53">
         <v>231</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I53">
+        <v>14.5</v>
+      </c>
+      <c r="J53">
+        <v>17.5</v>
+      </c>
+      <c r="K53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3761,8 +4383,20 @@
       <c r="G54">
         <v>231</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>23.6</v>
+      </c>
+      <c r="I54">
+        <v>18.2</v>
+      </c>
+      <c r="J54">
+        <v>23.6</v>
+      </c>
+      <c r="K54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -3781,8 +4415,20 @@
       <c r="G55">
         <v>231</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I55">
+        <v>25.7</v>
+      </c>
+      <c r="J55">
+        <v>31.2</v>
+      </c>
+      <c r="K55">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3801,8 +4447,20 @@
       <c r="G56">
         <v>231</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>22.6</v>
+      </c>
+      <c r="I56">
+        <v>18.2</v>
+      </c>
+      <c r="J56">
+        <v>19</v>
+      </c>
+      <c r="K56">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3821,8 +4479,20 @@
       <c r="G57">
         <v>231</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>27.2</v>
+      </c>
+      <c r="I57">
+        <v>22.1</v>
+      </c>
+      <c r="J57">
+        <v>25</v>
+      </c>
+      <c r="K57">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -3841,8 +4511,20 @@
       <c r="G58">
         <v>231</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <v>22</v>
+      </c>
+      <c r="I58">
+        <v>29.4</v>
+      </c>
+      <c r="J58">
+        <v>27.8</v>
+      </c>
+      <c r="K58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -3861,8 +4543,20 @@
       <c r="G59">
         <v>231</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>18.8</v>
+      </c>
+      <c r="I59">
+        <v>23.2</v>
+      </c>
+      <c r="J59">
+        <v>23</v>
+      </c>
+      <c r="K59">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -3881,8 +4575,20 @@
       <c r="G60">
         <v>231</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>28.3</v>
+      </c>
+      <c r="I60">
+        <v>29.9</v>
+      </c>
+      <c r="J60">
+        <v>35.9</v>
+      </c>
+      <c r="K60">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3901,8 +4607,20 @@
       <c r="G61">
         <v>231</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <v>21.3</v>
+      </c>
+      <c r="I61">
+        <v>25.1</v>
+      </c>
+      <c r="J61">
+        <v>29.2</v>
+      </c>
+      <c r="K61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -3921,8 +4639,20 @@
       <c r="G62">
         <v>231</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>24.1</v>
+      </c>
+      <c r="I62">
+        <v>28.5</v>
+      </c>
+      <c r="J62">
+        <v>28.5</v>
+      </c>
+      <c r="K62">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -3941,8 +4671,20 @@
       <c r="G63">
         <v>231</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <v>11.2</v>
+      </c>
+      <c r="I63">
+        <v>26.2</v>
+      </c>
+      <c r="J63">
+        <v>30.2</v>
+      </c>
+      <c r="K63">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3961,8 +4703,20 @@
       <c r="G64">
         <v>231</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <v>12.2</v>
+      </c>
+      <c r="I64">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="J64">
+        <v>21.3</v>
+      </c>
+      <c r="K64">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -3981,8 +4735,20 @@
       <c r="G65">
         <v>231</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <v>17.5</v>
+      </c>
+      <c r="I65">
+        <v>29.2</v>
+      </c>
+      <c r="J65">
+        <v>18</v>
+      </c>
+      <c r="K65">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -4001,8 +4767,20 @@
       <c r="G66">
         <v>231</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>20.2</v>
+      </c>
+      <c r="I66">
+        <v>22.8</v>
+      </c>
+      <c r="J66">
+        <v>18.3</v>
+      </c>
+      <c r="K66">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -4021,8 +4799,20 @@
       <c r="G67">
         <v>231</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>16.7</v>
+      </c>
+      <c r="I67">
+        <v>28.2</v>
+      </c>
+      <c r="J67">
+        <v>24.8</v>
+      </c>
+      <c r="K67">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -4041,8 +4831,20 @@
       <c r="G68">
         <v>231</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>17.7</v>
+      </c>
+      <c r="I68">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="J68">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K68">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -4061,8 +4863,20 @@
       <c r="G69">
         <v>231</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>24.4</v>
+      </c>
+      <c r="I69">
+        <v>22.8</v>
+      </c>
+      <c r="J69">
+        <v>23.2</v>
+      </c>
+      <c r="K69">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -4081,8 +4895,20 @@
       <c r="G70">
         <v>231</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>24.3</v>
+      </c>
+      <c r="I70">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J70">
+        <v>24.7</v>
+      </c>
+      <c r="K70">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -4101,8 +4927,20 @@
       <c r="G71">
         <v>231</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>28</v>
+      </c>
+      <c r="I71">
+        <v>23.4</v>
+      </c>
+      <c r="J71">
+        <v>26.6</v>
+      </c>
+      <c r="K71">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -4121,8 +4959,20 @@
       <c r="G72">
         <v>231</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>26.3</v>
+      </c>
+      <c r="I72">
+        <v>30.7</v>
+      </c>
+      <c r="J72">
+        <v>31.7</v>
+      </c>
+      <c r="K72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -4141,8 +4991,20 @@
       <c r="G73">
         <v>231</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="I73">
+        <v>28.6</v>
+      </c>
+      <c r="J73">
+        <v>19.3</v>
+      </c>
+      <c r="K73">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -4161,8 +5023,20 @@
       <c r="G74">
         <v>231</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>20.8</v>
+      </c>
+      <c r="I74">
+        <v>23.5</v>
+      </c>
+      <c r="J74">
+        <v>29.1</v>
+      </c>
+      <c r="K74">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -4181,8 +5055,20 @@
       <c r="G75">
         <v>231</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>34.5</v>
+      </c>
+      <c r="I75">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="J75">
+        <v>34</v>
+      </c>
+      <c r="K75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -4201,8 +5087,20 @@
       <c r="G76">
         <v>231</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H76">
+        <v>27.2</v>
+      </c>
+      <c r="I76">
+        <v>23.6</v>
+      </c>
+      <c r="J76">
+        <v>28.5</v>
+      </c>
+      <c r="K76">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -4221,8 +5119,20 @@
       <c r="G77">
         <v>231</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H77">
+        <v>25.8</v>
+      </c>
+      <c r="I77">
+        <v>27.1</v>
+      </c>
+      <c r="J77">
+        <v>28.4</v>
+      </c>
+      <c r="K77">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -4241,8 +5151,20 @@
       <c r="G78">
         <v>231</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>24.5</v>
+      </c>
+      <c r="I78">
+        <v>21.7</v>
+      </c>
+      <c r="J78">
+        <v>23.9</v>
+      </c>
+      <c r="K78">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -4261,8 +5183,20 @@
       <c r="G79">
         <v>231</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <v>14.5</v>
+      </c>
+      <c r="I79">
+        <v>18.3</v>
+      </c>
+      <c r="J79">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K79">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -4281,8 +5215,20 @@
       <c r="G80">
         <v>231</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>27.9</v>
+      </c>
+      <c r="I80">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="J80">
+        <v>22.2</v>
+      </c>
+      <c r="K80">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -4301,8 +5247,20 @@
       <c r="G81">
         <v>231</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>26.9</v>
+      </c>
+      <c r="I81">
+        <v>26.2</v>
+      </c>
+      <c r="J81">
+        <v>24</v>
+      </c>
+      <c r="K81">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -4321,8 +5279,20 @@
       <c r="G82">
         <v>231</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>24.5</v>
+      </c>
+      <c r="I82">
+        <v>27.7</v>
+      </c>
+      <c r="J82">
+        <v>26.4</v>
+      </c>
+      <c r="K82">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -4341,8 +5311,20 @@
       <c r="G83">
         <v>231</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I83">
+        <v>22.1</v>
+      </c>
+      <c r="J83">
+        <v>27</v>
+      </c>
+      <c r="K83">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -4361,8 +5343,20 @@
       <c r="G84">
         <v>231</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I84">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J84">
+        <v>19.5</v>
+      </c>
+      <c r="K84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -4381,8 +5375,20 @@
       <c r="G85">
         <v>231</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>30</v>
+      </c>
+      <c r="I85">
+        <v>20.3</v>
+      </c>
+      <c r="J85">
+        <v>19.8</v>
+      </c>
+      <c r="K85">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -4401,8 +5407,20 @@
       <c r="G86">
         <v>231</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>15.7</v>
+      </c>
+      <c r="I86">
+        <v>15.5</v>
+      </c>
+      <c r="J86">
+        <v>28</v>
+      </c>
+      <c r="K86">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -4421,8 +5439,20 @@
       <c r="G87">
         <v>231</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>22.5</v>
+      </c>
+      <c r="I87">
+        <v>25.2</v>
+      </c>
+      <c r="J87">
+        <v>29.5</v>
+      </c>
+      <c r="K87">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -4441,8 +5471,20 @@
       <c r="G88">
         <v>231</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H88">
+        <v>20.5</v>
+      </c>
+      <c r="I88">
+        <v>26</v>
+      </c>
+      <c r="J88">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K88">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -4461,8 +5503,20 @@
       <c r="G89">
         <v>231</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <v>10.4</v>
+      </c>
+      <c r="I89">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J89">
+        <v>31.6</v>
+      </c>
+      <c r="K89">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -4481,8 +5535,20 @@
       <c r="G90">
         <v>231</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>13</v>
+      </c>
+      <c r="I90">
+        <v>25.9</v>
+      </c>
+      <c r="J90">
+        <v>11.8</v>
+      </c>
+      <c r="K90">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -4500,6 +5566,18 @@
       </c>
       <c r="G91">
         <v>231</v>
+      </c>
+      <c r="H91">
+        <v>15.2</v>
+      </c>
+      <c r="I91">
+        <v>25.8</v>
+      </c>
+      <c r="J91">
+        <v>17.2</v>
+      </c>
+      <c r="K91">
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -4822,7 +5900,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -4841,20 +5919,20 @@
       <c r="G102">
         <v>231</v>
       </c>
-      <c r="H102" s="1">
+      <c r="H102">
         <v>20.399999999999999</v>
       </c>
-      <c r="I102" s="1">
+      <c r="I102">
         <v>25.6</v>
       </c>
-      <c r="J102" s="1">
+      <c r="J102">
         <v>23.7</v>
       </c>
-      <c r="K102" s="1">
+      <c r="K102">
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -4873,20 +5951,20 @@
       <c r="G103">
         <v>231</v>
       </c>
-      <c r="H103" s="1">
+      <c r="H103">
         <v>15.6</v>
       </c>
-      <c r="I103" s="1">
+      <c r="I103">
         <v>22.2</v>
       </c>
-      <c r="J103" s="1">
+      <c r="J103">
         <v>22.9</v>
       </c>
-      <c r="K103" s="1">
+      <c r="K103">
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -4905,20 +5983,20 @@
       <c r="G104">
         <v>231</v>
       </c>
-      <c r="H104" s="1">
+      <c r="H104">
         <v>14.4</v>
       </c>
-      <c r="I104" s="1">
+      <c r="I104">
         <v>24.8</v>
       </c>
-      <c r="J104" s="1">
+      <c r="J104">
         <v>34</v>
       </c>
-      <c r="K104" s="1">
+      <c r="K104">
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -4937,20 +6015,20 @@
       <c r="G105">
         <v>231</v>
       </c>
-      <c r="H105" s="1">
+      <c r="H105">
         <v>19.3</v>
       </c>
-      <c r="I105" s="1">
+      <c r="I105">
         <v>24</v>
       </c>
-      <c r="J105" s="1">
+      <c r="J105">
         <v>34.299999999999997</v>
       </c>
-      <c r="K105" s="1">
+      <c r="K105">
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -4969,16 +6047,16 @@
       <c r="G106">
         <v>231</v>
       </c>
-      <c r="H106" s="1">
+      <c r="H106">
         <v>19.100000000000001</v>
       </c>
-      <c r="I106" s="1">
+      <c r="I106">
         <v>19.600000000000001</v>
       </c>
-      <c r="J106" s="1">
+      <c r="J106">
         <v>21.8</v>
       </c>
-      <c r="K106" s="1">
+      <c r="K106">
         <v>90</v>
       </c>
     </row>
@@ -5302,7 +6380,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -5334,7 +6412,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -5366,7 +6444,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -5398,7 +6476,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -5430,7 +6508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -5782,7 +6860,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -5814,7 +6892,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -5846,7 +6924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -5878,7 +6956,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -5910,7 +6988,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -6121,16 +7199,16 @@
       <c r="G142">
         <v>231</v>
       </c>
-      <c r="H142" s="1">
+      <c r="H142">
         <v>26.2</v>
       </c>
-      <c r="I142" s="1">
+      <c r="I142">
         <v>22.6</v>
       </c>
-      <c r="J142" s="1">
+      <c r="J142">
         <v>17.8</v>
       </c>
-      <c r="K142" s="1">
+      <c r="K142">
         <v>90</v>
       </c>
     </row>
@@ -6153,16 +7231,16 @@
       <c r="G143">
         <v>231</v>
       </c>
-      <c r="H143" s="1">
+      <c r="H143">
         <v>23.9</v>
       </c>
-      <c r="I143" s="1">
+      <c r="I143">
         <v>19.5</v>
       </c>
-      <c r="J143" s="1">
+      <c r="J143">
         <v>23.7</v>
       </c>
-      <c r="K143" s="1">
+      <c r="K143">
         <v>90</v>
       </c>
     </row>
@@ -6185,16 +7263,16 @@
       <c r="G144">
         <v>231</v>
       </c>
-      <c r="H144" s="1">
+      <c r="H144">
         <v>21.4</v>
       </c>
-      <c r="I144" s="1">
+      <c r="I144">
         <v>22.9</v>
       </c>
-      <c r="J144" s="1">
+      <c r="J144">
         <v>40.799999999999997</v>
       </c>
-      <c r="K144" s="1">
+      <c r="K144">
         <v>90</v>
       </c>
     </row>
@@ -6217,16 +7295,16 @@
       <c r="G145">
         <v>231</v>
       </c>
-      <c r="H145" s="1">
+      <c r="H145">
         <v>22.2</v>
       </c>
-      <c r="I145" s="1">
+      <c r="I145">
         <v>14.8</v>
       </c>
-      <c r="J145" s="1">
+      <c r="J145">
         <v>38.6</v>
       </c>
-      <c r="K145" s="1">
+      <c r="K145">
         <v>80</v>
       </c>
     </row>
@@ -6249,20 +7327,20 @@
       <c r="G146">
         <v>231</v>
       </c>
-      <c r="H146" s="1">
+      <c r="H146">
         <v>35.299999999999997</v>
       </c>
-      <c r="I146" s="1">
+      <c r="I146">
         <v>29.2</v>
       </c>
-      <c r="J146" s="1">
+      <c r="J146">
         <v>38.5</v>
       </c>
-      <c r="K146" s="1">
+      <c r="K146">
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -6294,7 +7372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -6326,7 +7404,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -6358,7 +7436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -6390,7 +7468,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -6742,7 +7820,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -6774,7 +7852,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -6806,7 +7884,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -6838,7 +7916,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -6870,7 +7948,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -6898,8 +7976,8 @@
       <c r="J166">
         <v>26.3</v>
       </c>
-      <c r="K166">
-        <v>90</v>
+      <c r="K166" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -7222,7 +8300,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -7254,7 +8332,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -7286,7 +8364,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -7318,7 +8396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -7350,7 +8428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -11004,16 +12082,16 @@
       <c r="G326">
         <v>231</v>
       </c>
-      <c r="H326" s="1">
+      <c r="H326">
         <v>31.8</v>
       </c>
-      <c r="I326" s="1">
+      <c r="I326">
         <v>28.9</v>
       </c>
-      <c r="J326" s="1">
+      <c r="J326">
         <v>24.7</v>
       </c>
-      <c r="K326" s="1">
+      <c r="K326">
         <v>95</v>
       </c>
     </row>
@@ -11036,16 +12114,16 @@
       <c r="G327">
         <v>231</v>
       </c>
-      <c r="H327" s="1">
+      <c r="H327">
         <v>26</v>
       </c>
-      <c r="I327" s="1">
+      <c r="I327">
         <v>26</v>
       </c>
-      <c r="J327" s="1">
+      <c r="J327">
         <v>31.3</v>
       </c>
-      <c r="K327" s="1">
+      <c r="K327">
         <v>90</v>
       </c>
     </row>
@@ -11068,16 +12146,16 @@
       <c r="G328">
         <v>231</v>
       </c>
-      <c r="H328" s="1">
+      <c r="H328">
         <v>28.3</v>
       </c>
-      <c r="I328" s="1">
+      <c r="I328">
         <v>22.7</v>
       </c>
-      <c r="J328" s="1">
+      <c r="J328">
         <v>23.1</v>
       </c>
-      <c r="K328" s="1">
+      <c r="K328">
         <v>95</v>
       </c>
     </row>

</xml_diff>